<commit_message>
Processed Macro Scenario Information
</commit_message>
<xml_diff>
--- a/data/sam/GEO_Macro_varlist.xlsx
+++ b/data/sam/GEO_Macro_varlist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -52,13 +52,13 @@
     <t xml:space="preserve">Population (million)</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_m</t>
+    <t xml:space="preserve">population_m</t>
   </si>
   <si>
     <t xml:space="preserve">Working age Population (million)</t>
   </si>
   <si>
-    <t xml:space="preserve">work_age_pop_m</t>
+    <t xml:space="preserve">working_age_pop_m</t>
   </si>
   <si>
     <t xml:space="preserve">Employment (headcounts, mil)</t>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t xml:space="preserve">epi_h-hh5_urb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario Id.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario_id</t>
   </si>
 </sst>
 </file>
@@ -301,6 +307,7 @@
       <sz val="10"/>
       <name val="Aptos"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -365,7 +372,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,10 +499,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.96484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -509,7 +516,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -525,8 +532,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1039,6 +1045,15 @@
       <c r="C51" s="1" t="s">
         <v>88</v>
       </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>